<commit_message>
Added My Timesheets and New Folders
</commit_message>
<xml_diff>
--- a/0201_0207/JaredKeefer.xlsx
+++ b/0201_0207/JaredKeefer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Classes\Capstone\Project\GitRepo\bison-timesheets\0131_0206\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Classes\Capstone\Project\GitRepo\bison-timesheets\0201_0207\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEFC7851-1747-4165-B899-6E50AC999CEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D2CCCF-F3AB-4ADB-844B-2E99535D23B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1950" windowWidth="21600" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="2295" windowWidth="21600" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,25 +573,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="12">
-        <v>44227</v>
+        <v>44228</v>
       </c>
       <c r="C5" s="12">
-        <v>44228</v>
+        <v>44229</v>
       </c>
       <c r="D5" s="12">
-        <v>44229</v>
+        <v>44230</v>
       </c>
       <c r="E5" s="12">
-        <v>44230</v>
+        <v>44231</v>
       </c>
       <c r="F5" s="12">
-        <v>44231</v>
+        <v>44232</v>
       </c>
       <c r="G5" s="12">
-        <v>44232</v>
+        <v>44233</v>
       </c>
       <c r="H5" s="13">
-        <v>44233</v>
+        <v>44234</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>5</v>

</xml_diff>